<commit_message>
add memory layout diagram
</commit_message>
<xml_diff>
--- a/files/内存分布.xlsx
+++ b/files/内存分布.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/libinyl/Documents/GitHub/6828/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2180F8B5-8E5F-3B46-ABA2-9B30BC6D602C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA47ADBA-88C2-FD4D-A2F9-04759B9BA0F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{31FFD905-892E-7D47-A442-CC69616C68DF}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{31FFD905-892E-7D47-A442-CC69616C68DF}"/>
   </bookViews>
   <sheets>
     <sheet name="lab1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'lab2'!$A$2:$K$31</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -805,7 +804,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -990,6 +989,11 @@
       <sz val="8"/>
       <color theme="1"/>
       <name val="等线 (正文)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="27">
@@ -1266,7 +1270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1557,6 +1561,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1569,113 +1660,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2696,8 +2706,8 @@
   </sheetPr>
   <dimension ref="A1:S84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="229" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="57" zoomScaleNormal="229" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2710,7 +2720,7 @@
     <col min="6" max="6" width="4.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="2" style="31" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="21.83203125" style="22" customWidth="1"/>
     <col min="10" max="10" width="29.5" style="2" customWidth="1"/>
     <col min="11" max="11" width="10.1640625" style="31" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" style="1" customWidth="1"/>
@@ -2729,20 +2739,20 @@
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98" t="s">
+      <c r="C1" s="127" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
       <c r="G1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="120" t="s">
+      <c r="H1" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="120"/>
-      <c r="J1" s="18" t="s">
+      <c r="I1" s="109"/>
+      <c r="J1" s="139" t="s">
         <v>97</v>
       </c>
       <c r="K1" s="3"/>
@@ -2752,30 +2762,30 @@
       <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
       <c r="G2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
     </row>
     <row r="3" spans="1:19" s="2" customFormat="1" ht="41" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="110" t="s">
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
       <c r="K3" s="31"/>
       <c r="L3" s="16" t="s">
         <v>73</v>
@@ -2794,11 +2804,11 @@
       <c r="B4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="110"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="134"/>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
       <c r="J4" s="36"/>
@@ -2820,11 +2830,11 @@
       <c r="B5" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="110"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="134"/>
       <c r="H5" s="94"/>
       <c r="I5" s="30"/>
       <c r="J5" s="37" t="s">
@@ -2850,11 +2860,11 @@
       <c r="B6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="110"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="134"/>
       <c r="H6" s="94"/>
       <c r="I6" s="30"/>
       <c r="L6" s="4"/>
@@ -2864,17 +2874,17 @@
     <row r="7" spans="1:19" s="2" customFormat="1" ht="120" customHeight="1" thickBot="1">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="101" t="s">
+      <c r="C7" s="129"/>
+      <c r="D7" s="129"/>
+      <c r="E7" s="129"/>
+      <c r="F7" s="129"/>
+      <c r="G7" s="130" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="137" t="s">
+      <c r="H7" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="137"/>
+      <c r="I7" s="123"/>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16" t="s">
@@ -2892,18 +2902,18 @@
     <row r="8" spans="1:19" s="4" customFormat="1" ht="59" customHeight="1" thickTop="1">
       <c r="A8" s="7"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="135" t="s">
+      <c r="C8" s="129"/>
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="130"/>
+      <c r="H8" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="I8" s="135"/>
+      <c r="I8" s="121"/>
       <c r="J8"/>
       <c r="K8" s="64"/>
-      <c r="L8" s="103" t="s">
+      <c r="L8" s="131" t="s">
         <v>76</v>
       </c>
       <c r="M8" s="31"/>
@@ -2912,14 +2922,14 @@
     <row r="9" spans="1:19" s="4" customFormat="1" ht="21" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="136"/>
-      <c r="I9" s="136"/>
-      <c r="L9" s="103"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="130"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="122"/>
+      <c r="L9" s="131"/>
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>
       <c r="O9" s="61" t="s">
@@ -2939,23 +2949,23 @@
     <row r="10" spans="1:19" s="2" customFormat="1" ht="13" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="136"/>
-      <c r="I10" s="136"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="122"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="103"/>
+      <c r="L10" s="131"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="P10" s="114"/>
-      <c r="Q10" s="114"/>
-      <c r="R10" s="115" t="s">
+      <c r="P10" s="125"/>
+      <c r="Q10" s="125"/>
+      <c r="R10" s="111" t="s">
         <v>68</v>
       </c>
       <c r="S10" s="12"/>
@@ -2963,75 +2973,75 @@
     <row r="11" spans="1:19" s="31" customFormat="1" ht="51" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="133" t="s">
+      <c r="C11" s="129"/>
+      <c r="D11" s="129"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="129"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="120" t="s">
         <v>114</v>
       </c>
-      <c r="I11" s="133"/>
+      <c r="I11" s="120"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="103"/>
+      <c r="L11" s="131"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="P11" s="129" t="s">
+      <c r="P11" s="106" t="s">
         <v>62</v>
       </c>
-      <c r="Q11" s="102" t="s">
+      <c r="Q11" s="110" t="s">
         <v>115</v>
       </c>
-      <c r="R11" s="115"/>
+      <c r="R11" s="111"/>
       <c r="S11" s="10"/>
     </row>
     <row r="12" spans="1:19" s="31" customFormat="1" ht="57" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="127"/>
-      <c r="I12" s="126" t="s">
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="104"/>
+      <c r="I12" s="103" t="s">
         <v>117</v>
       </c>
-      <c r="J12" s="130" t="s">
+      <c r="J12" s="107" t="s">
         <v>110</v>
       </c>
       <c r="K12" s="4"/>
-      <c r="L12" s="103"/>
+      <c r="L12" s="131"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12"/>
-      <c r="P12" s="129"/>
-      <c r="Q12" s="102"/>
-      <c r="R12" s="115"/>
+      <c r="P12" s="106"/>
+      <c r="Q12" s="110"/>
+      <c r="R12" s="111"/>
     </row>
     <row r="13" spans="1:19" s="31" customFormat="1" ht="21" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="132" t="s">
+      <c r="C13" s="129"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="114" t="s">
         <v>113</v>
       </c>
-      <c r="I13" s="132"/>
-      <c r="J13" s="134"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="108"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="103"/>
+      <c r="L13" s="131"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="P13" s="129"/>
-      <c r="Q13" s="102"/>
-      <c r="R13" s="115"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="110"/>
+      <c r="R13" s="111"/>
       <c r="S13" s="44" t="s">
         <v>63</v>
       </c>
@@ -3039,24 +3049,24 @@
     <row r="14" spans="1:19" s="31" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="132"/>
-      <c r="J14" s="128"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="129"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="114"/>
+      <c r="I14" s="114"/>
+      <c r="J14" s="105"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="103"/>
+      <c r="L14" s="131"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="P14" s="129"/>
+      <c r="P14" s="106"/>
       <c r="Q14" s="88"/>
-      <c r="R14" s="115"/>
+      <c r="R14" s="111"/>
       <c r="S14" s="45"/>
     </row>
     <row r="15" spans="1:19" ht="29" customHeight="1">
@@ -3066,28 +3076,28 @@
       <c r="B15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="131" t="s">
+      <c r="C15" s="129"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="119" t="s">
         <v>112</v>
       </c>
-      <c r="I15" s="131"/>
+      <c r="I15" s="119"/>
       <c r="J15" s="13" t="s">
         <v>54</v>
       </c>
       <c r="K15" s="10"/>
-      <c r="L15" s="103"/>
+      <c r="L15" s="131"/>
       <c r="O15" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="P15" s="129"/>
+      <c r="P15" s="106"/>
       <c r="Q15" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="R15" s="115"/>
+      <c r="R15" s="111"/>
       <c r="S15" s="46" t="s">
         <v>45</v>
       </c>
@@ -3097,24 +3107,24 @@
       <c r="B16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="111" t="s">
+      <c r="C16" s="116" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="100" t="s">
+      <c r="F16" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="112" t="s">
+      <c r="G16" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="107" t="s">
+      <c r="H16" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="107"/>
+      <c r="I16" s="118"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
-      <c r="L16" s="103"/>
+      <c r="L16" s="131"/>
       <c r="M16" s="31"/>
       <c r="N16" s="31"/>
       <c r="O16" s="43" t="s">
@@ -3122,7 +3132,7 @@
       </c>
       <c r="P16" s="88"/>
       <c r="Q16" s="88"/>
-      <c r="R16" s="115"/>
+      <c r="R16" s="111"/>
       <c r="S16" s="51" t="s">
         <v>60</v>
       </c>
@@ -3132,26 +3142,26 @@
       <c r="B17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="111"/>
+      <c r="C17" s="116"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="108" t="s">
+      <c r="E17" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="100"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
+      <c r="F17" s="129"/>
+      <c r="G17" s="135"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
-      <c r="L17" s="103"/>
+      <c r="L17" s="131"/>
       <c r="O17" s="42"/>
       <c r="P17" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="Q17" s="118" t="s">
+      <c r="Q17" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="R17" s="115"/>
+      <c r="R17" s="111"/>
       <c r="S17" s="45"/>
     </row>
     <row r="18" spans="1:19" ht="33" customHeight="1">
@@ -3161,24 +3171,24 @@
       <c r="B18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="108"/>
-      <c r="F18" s="100"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="129"/>
       <c r="G18" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
-      <c r="L18" s="103"/>
+      <c r="L18" s="131"/>
       <c r="O18" s="43" t="s">
         <v>38</v>
       </c>
       <c r="P18" s="89"/>
-      <c r="Q18" s="118"/>
-      <c r="R18" s="115"/>
+      <c r="Q18" s="126"/>
+      <c r="R18" s="111"/>
       <c r="S18" s="44" t="s">
         <v>44</v>
       </c>
@@ -3186,18 +3196,18 @@
     <row r="19" spans="1:19" s="2" customFormat="1" ht="17" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="101" t="s">
+      <c r="C19" s="132"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="129"/>
+      <c r="G19" s="130" t="s">
         <v>118</v>
       </c>
       <c r="H19" s="32"/>
       <c r="I19" s="32"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
-      <c r="L19" s="103"/>
+      <c r="L19" s="131"/>
       <c r="M19" s="31"/>
       <c r="N19" s="31"/>
       <c r="O19" s="31"/>
@@ -3205,49 +3215,49 @@
       <c r="Q19" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="R19" s="115"/>
+      <c r="R19" s="111"/>
       <c r="S19" s="45"/>
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="109" t="s">
+      <c r="C20" s="132"/>
+      <c r="D20" s="132"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="130"/>
+      <c r="H20" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="I20" s="109"/>
+      <c r="I20" s="117"/>
       <c r="J20" s="27" t="s">
         <v>55</v>
       </c>
       <c r="K20" s="65"/>
-      <c r="L20" s="103"/>
+      <c r="L20" s="131"/>
       <c r="M20" s="31"/>
       <c r="N20" s="31"/>
       <c r="O20" s="42"/>
       <c r="P20" s="89"/>
       <c r="Q20" s="93"/>
-      <c r="R20" s="115"/>
+      <c r="R20" s="111"/>
       <c r="S20" s="45"/>
     </row>
     <row r="21" spans="1:19" s="2" customFormat="1" ht="14" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="101"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="129"/>
+      <c r="G21" s="130"/>
       <c r="H21" s="32"/>
       <c r="I21" s="28"/>
       <c r="J21" s="27" t="s">
         <v>48</v>
       </c>
       <c r="K21" s="65"/>
-      <c r="L21" s="103"/>
+      <c r="L21" s="131"/>
       <c r="M21" s="31"/>
       <c r="N21" s="31"/>
       <c r="O21" s="43" t="s">
@@ -3255,7 +3265,7 @@
       </c>
       <c r="P21" s="89"/>
       <c r="Q21" s="93"/>
-      <c r="R21" s="115"/>
+      <c r="R21" s="111"/>
       <c r="S21" s="44" t="s">
         <v>43</v>
       </c>
@@ -3263,44 +3273,44 @@
     <row r="22" spans="1:19" s="2" customFormat="1" ht="16" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="111" t="s">
+      <c r="C22" s="132"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="129"/>
+      <c r="G22" s="130"/>
+      <c r="H22" s="116" t="s">
         <v>49</v>
       </c>
-      <c r="I22" s="111"/>
+      <c r="I22" s="116"/>
       <c r="J22" s="13" t="s">
         <v>19</v>
       </c>
       <c r="K22" s="10"/>
-      <c r="L22" s="103"/>
+      <c r="L22" s="131"/>
       <c r="N22" s="31"/>
       <c r="O22" s="41" t="s">
         <v>39</v>
       </c>
       <c r="P22" s="89"/>
       <c r="Q22" s="88"/>
-      <c r="R22" s="115"/>
+      <c r="R22" s="111"/>
       <c r="S22" s="45"/>
     </row>
     <row r="23" spans="1:19" s="31" customFormat="1" ht="19" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="132" t="s">
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="130"/>
+      <c r="H23" s="114" t="s">
         <v>119</v>
       </c>
-      <c r="I23" s="113"/>
+      <c r="I23" s="115"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="103"/>
+      <c r="L23" s="131"/>
       <c r="M23" s="5" t="s">
         <v>75</v>
       </c>
@@ -3309,7 +3319,7 @@
       <c r="Q23" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="R23" s="115"/>
+      <c r="R23" s="111"/>
       <c r="S23" s="45"/>
     </row>
     <row r="24" spans="1:19" ht="18" customHeight="1">
@@ -3317,16 +3327,16 @@
       <c r="B24" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="113"/>
-      <c r="I24" s="113"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="130"/>
+      <c r="H24" s="115"/>
+      <c r="I24" s="115"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="103"/>
+      <c r="L24" s="131"/>
       <c r="M24" s="5">
         <v>0</v>
       </c>
@@ -3335,7 +3345,7 @@
       </c>
       <c r="P24" s="89"/>
       <c r="Q24" s="90"/>
-      <c r="R24" s="115"/>
+      <c r="R24" s="111"/>
       <c r="S24" s="44" t="s">
         <v>42</v>
       </c>
@@ -3346,7 +3356,7 @@
       </c>
       <c r="P25" s="89"/>
       <c r="Q25" s="88"/>
-      <c r="R25" s="115"/>
+      <c r="R25" s="111"/>
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:19">
@@ -3357,7 +3367,7 @@
       <c r="Q26" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="R26" s="115"/>
+      <c r="R26" s="111"/>
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:19" ht="17">
@@ -3366,7 +3376,7 @@
       </c>
       <c r="P27" s="89"/>
       <c r="Q27" s="91"/>
-      <c r="R27" s="115"/>
+      <c r="R27" s="111"/>
       <c r="S27" s="47" t="s">
         <v>58</v>
       </c>
@@ -3375,35 +3385,35 @@
       <c r="O28" s="31"/>
       <c r="P28" s="88"/>
       <c r="Q28" s="88"/>
-      <c r="R28" s="115"/>
+      <c r="R28" s="111"/>
       <c r="S28" s="53"/>
     </row>
     <row r="29" spans="1:19">
       <c r="O29" s="31"/>
-      <c r="P29" s="93" t="s">
+      <c r="P29" s="138" t="s">
         <v>59</v>
       </c>
-      <c r="Q29" s="93"/>
-      <c r="R29" s="115"/>
+      <c r="Q29" s="138"/>
+      <c r="R29" s="111"/>
       <c r="S29" s="53"/>
     </row>
     <row r="30" spans="1:19" ht="18" thickBot="1">
       <c r="O30" s="25"/>
-      <c r="P30" s="117" t="s">
+      <c r="P30" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="Q30" s="117"/>
-      <c r="R30" s="116"/>
+      <c r="Q30" s="124"/>
+      <c r="R30" s="112"/>
       <c r="S30" s="54" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="17" thickTop="1">
       <c r="O31" s="25"/>
-      <c r="P31" s="111" t="s">
+      <c r="P31" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="Q31" s="111"/>
+      <c r="Q31" s="116"/>
       <c r="R31" s="55" t="s">
         <v>64</v>
       </c>
@@ -3948,20 +3958,9 @@
       <c r="S84"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="Q11:Q13"/>
-    <mergeCell ref="R10:R30"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H23:I24"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H16:I18"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H13:I14"/>
-    <mergeCell ref="H8:I10"/>
-    <mergeCell ref="H7:I7"/>
+  <mergeCells count="31">
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="P29:Q29"/>
     <mergeCell ref="P31:Q31"/>
     <mergeCell ref="P30:Q30"/>
     <mergeCell ref="P10:Q10"/>
@@ -3978,11 +3977,23 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="G3:G6"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="Q11:Q13"/>
+    <mergeCell ref="R10:R30"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H16:I18"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I14"/>
+    <mergeCell ref="H8:I10"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="49" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="38" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
@@ -3995,8 +4006,8 @@
   </sheetPr>
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="84" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="84" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4018,7 +4029,7 @@
       <c r="A1" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="109" t="s">
         <v>96</v>
       </c>
       <c r="C1" s="76" t="s">
@@ -4029,7 +4040,7 @@
       <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="120"/>
+      <c r="B2" s="109"/>
       <c r="C2" s="85"/>
       <c r="D2" s="3"/>
     </row>
@@ -4037,11 +4048,11 @@
       <c r="A3" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="106"/>
+      <c r="B3" s="113"/>
     </row>
     <row r="4" spans="1:11" ht="41" customHeight="1">
       <c r="A4" s="71"/>
-      <c r="B4" s="106"/>
+      <c r="B4" s="113"/>
       <c r="E4" s="16" t="s">
         <v>73</v>
       </c>
@@ -4066,7 +4077,7 @@
       <c r="G5"/>
     </row>
     <row r="6" spans="1:11" ht="16" customHeight="1">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="102" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="58"/>
@@ -4081,7 +4092,7 @@
       <c r="G6"/>
     </row>
     <row r="7" spans="1:11" ht="119" customHeight="1" thickBot="1">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="101" t="s">
         <v>106</v>
       </c>
       <c r="B7" s="58"/>
@@ -4090,7 +4101,7 @@
     </row>
     <row r="8" spans="1:11" ht="120" customHeight="1">
       <c r="A8" s="71"/>
-      <c r="B8" s="121"/>
+      <c r="B8" s="98"/>
       <c r="C8" s="13" t="s">
         <v>14</v>
       </c>
@@ -4108,9 +4119,9 @@
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="52" customHeight="1">
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A10" s="70"/>
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="99" t="s">
         <v>105</v>
       </c>
       <c r="C10" s="10"/>
@@ -4120,7 +4131,7 @@
       <c r="J10"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="60" customHeight="1">
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="41" customHeight="1">
       <c r="A11" s="70"/>
       <c r="B11" s="29" t="s">
         <v>103</v>
@@ -4151,7 +4162,7 @@
     </row>
     <row r="13" spans="1:11" ht="12" customHeight="1">
       <c r="A13" s="70"/>
-      <c r="B13" s="102" t="s">
+      <c r="B13" s="110" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="81" t="s">
@@ -4165,7 +4176,7 @@
     </row>
     <row r="14" spans="1:11" ht="14" customHeight="1">
       <c r="A14" s="70"/>
-      <c r="B14" s="102"/>
+      <c r="B14" s="110"/>
       <c r="C14" s="84" t="s">
         <v>99</v>
       </c>
@@ -4177,12 +4188,12 @@
     </row>
     <row r="15" spans="1:11" ht="136" customHeight="1">
       <c r="A15" s="70"/>
-      <c r="B15" s="102"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="82" t="s">
         <v>83</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="F15" s="123" t="s">
+      <c r="F15" s="100" t="s">
         <v>104</v>
       </c>
       <c r="I15"/>
@@ -4190,7 +4201,7 @@
       <c r="K15"/>
     </row>
     <row r="16" spans="1:11" ht="37" customHeight="1">
-      <c r="A16" s="124" t="s">
+      <c r="A16" s="101" t="s">
         <v>107</v>
       </c>
       <c r="B16" s="68" t="s">
@@ -4205,7 +4216,7 @@
       <c r="K16"/>
     </row>
     <row r="17" spans="1:11" ht="51" customHeight="1">
-      <c r="A17" s="124" t="s">
+      <c r="A17" s="101" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="95" t="s">
@@ -4355,7 +4366,7 @@
     </row>
     <row r="46" spans="7:12">
       <c r="K46" s="39"/>
-      <c r="L46" s="102" t="s">
+      <c r="L46" s="110" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4363,7 +4374,7 @@
       <c r="K47" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="L47" s="102"/>
+      <c r="L47" s="110"/>
     </row>
     <row r="48" spans="7:12">
       <c r="K48" s="41" t="s">
@@ -4373,7 +4384,7 @@
     </row>
     <row r="49" spans="2:12">
       <c r="K49" s="42"/>
-      <c r="L49" s="103" t="s">
+      <c r="L49" s="131" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4388,7 +4399,7 @@
       <c r="K50" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="L50" s="104"/>
+      <c r="L50" s="136"/>
     </row>
     <row r="51" spans="2:12">
       <c r="B51"/>
@@ -4412,7 +4423,7 @@
       <c r="G52"/>
       <c r="H52"/>
       <c r="K52" s="42"/>
-      <c r="L52" s="118" t="s">
+      <c r="L52" s="126" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4425,7 +4436,7 @@
       <c r="G53"/>
       <c r="H53"/>
       <c r="K53" s="42"/>
-      <c r="L53" s="118"/>
+      <c r="L53" s="126"/>
     </row>
     <row r="54" spans="2:12">
       <c r="B54"/>
@@ -4438,7 +4449,7 @@
       <c r="K54" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="L54" s="118"/>
+      <c r="L54" s="126"/>
     </row>
     <row r="55" spans="2:12">
       <c r="B55"/>
@@ -4484,7 +4495,7 @@
     </row>
     <row r="60" spans="2:12">
       <c r="K60" s="42"/>
-      <c r="L60" s="119" t="s">
+      <c r="L60" s="137" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4492,7 +4503,7 @@
       <c r="K61" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="L61" s="119"/>
+      <c r="L61" s="137"/>
     </row>
     <row r="62" spans="2:12">
       <c r="K62" s="41" t="s">
@@ -4504,7 +4515,7 @@
       <c r="K63" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="L63" s="104" t="s">
+      <c r="L63" s="136" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4512,18 +4523,18 @@
       <c r="K64" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="L64" s="104"/>
+      <c r="L64" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="L52:L54"/>
+    <mergeCell ref="L60:L61"/>
+    <mergeCell ref="L63:L64"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="L46:L47"/>
     <mergeCell ref="L49:L50"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="L52:L54"/>
-    <mergeCell ref="L60:L61"/>
-    <mergeCell ref="L63:L64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>